<commit_message>
Début de vérification global de style.css
</commit_message>
<xml_diff>
--- a/docs/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
+++ b/docs/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t xml:space="preserve">Categorie</t>
   </si>
@@ -161,6 +161,21 @@
   </si>
   <si>
     <t xml:space="preserve">codé le CSS en mobile first, meilleur utilisation des breakpoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Favico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utiliser image ,ico, ,png, ,svg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">image au format jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modifier l’image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://facemweb.com/creation-web/favicon-definition</t>
   </si>
   <si>
     <t xml:space="preserve">Structure</t>
@@ -375,7 +390,7 @@
   <dimension ref="A1:Z23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -578,12 +593,29 @@
         <v>46</v>
       </c>
     </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -593,16 +625,16 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Refonte du site en bootstrap 4 - Utilisation de sass
</commit_message>
<xml_diff>
--- a/docs/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
+++ b/docs/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
@@ -209,6 +209,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -231,6 +232,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -238,11 +240,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -387,18 +391,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z23"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="48.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="48.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="47.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="10.56"/>

</xml_diff>

<commit_message>
Modification des images, mise en place google maps
</commit_message>
<xml_diff>
--- a/docs/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
+++ b/docs/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t xml:space="preserve">Categorie</t>
   </si>
@@ -163,19 +163,25 @@
     <t xml:space="preserve">codé le CSS en mobile first, meilleur utilisation des breakpoint</t>
   </si>
   <si>
+    <t xml:space="preserve">https://webmasters.googleblog.com/2016/11/mobile-first-indexing.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">Favico</t>
   </si>
   <si>
-    <t xml:space="preserve">Utiliser image ,ico, ,png, ,svg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">image au format jpeg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modifier l’image</t>
+    <t xml:space="preserve">Utiliser images ,ico, ,png, ,svg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">images au format jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modifier les images</t>
   </si>
   <si>
     <t xml:space="preserve">https://facemweb.com/creation-web/favicon-definition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.lafabriquedunet.fr/creation-site-vitrine/articles/optimiser-images-web/</t>
   </si>
   <si>
     <t xml:space="preserve">Structure</t>
@@ -393,17 +399,17 @@
   </sheetPr>
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="48.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="47.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="52.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="64.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="70.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="10.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="27" style="0" width="11.22"/>
@@ -596,30 +602,38 @@
       <c r="E17" s="0" t="s">
         <v>46</v>
       </c>
+      <c r="F17" s="0" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F19" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -629,16 +643,16 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>